<commit_message>
Updated Database - coordinates
coordinates of stops on 27 to and from and 77a to Job
</commit_message>
<xml_diff>
--- a/27 From Clare Hall to Jobstown.xlsx
+++ b/27 From Clare Hall to Jobstown.xlsx
@@ -427,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +442,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -464,9 +470,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1198,7 +1205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="3:6">
+    <row r="33" spans="1:6">
       <c r="C33">
         <v>27</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="3:6">
+    <row r="34" spans="1:6">
       <c r="C34">
         <v>27</v>
       </c>
@@ -1226,7 +1233,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="3:6">
+    <row r="35" spans="1:6">
       <c r="C35">
         <v>27</v>
       </c>
@@ -1240,7 +1247,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="3:6">
+    <row r="36" spans="1:6">
       <c r="C36">
         <v>27</v>
       </c>
@@ -1254,7 +1261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="3:6">
+    <row r="37" spans="1:6">
       <c r="C37">
         <v>27</v>
       </c>
@@ -1268,7 +1275,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="3:6">
+    <row r="38" spans="1:6">
       <c r="C38">
         <v>27</v>
       </c>
@@ -1282,7 +1289,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="3:6">
+    <row r="39" spans="1:6">
       <c r="C39">
         <v>27</v>
       </c>
@@ -1296,7 +1303,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="3:6">
+    <row r="40" spans="1:6">
       <c r="C40">
         <v>27</v>
       </c>
@@ -1310,7 +1317,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="3:6">
+    <row r="41" spans="1:6">
       <c r="C41">
         <v>27</v>
       </c>
@@ -1324,7 +1331,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="3:6">
+    <row r="42" spans="1:6">
       <c r="C42">
         <v>27</v>
       </c>
@@ -1338,7 +1345,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="3:6">
+    <row r="43" spans="1:6">
       <c r="C43">
         <v>27</v>
       </c>
@@ -1352,7 +1359,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="3:6">
+    <row r="44" spans="1:6">
       <c r="C44">
         <v>27</v>
       </c>
@@ -1366,7 +1373,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="3:6">
+    <row r="45" spans="1:6">
       <c r="C45">
         <v>27</v>
       </c>
@@ -1380,7 +1387,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="3:6">
+    <row r="46" spans="1:6">
       <c r="C46">
         <v>27</v>
       </c>
@@ -1394,7 +1401,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="3:6">
+    <row r="47" spans="1:6" ht="15.75">
+      <c r="A47" s="2">
+        <v>53.344290999999998</v>
+      </c>
+      <c r="B47" s="2">
+        <v>-6.2656140000000002</v>
+      </c>
       <c r="C47">
         <v>27</v>
       </c>
@@ -1408,7 +1421,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="3:6">
+    <row r="48" spans="1:6" ht="15.75">
+      <c r="A48" s="2">
+        <v>53.342447999999997</v>
+      </c>
+      <c r="B48">
+        <v>-6.2697950000000002</v>
+      </c>
       <c r="C48">
         <v>27</v>
       </c>
@@ -1422,7 +1441,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="3:6">
+    <row r="49" spans="1:6" ht="15.75">
+      <c r="A49" s="2">
+        <v>53.338182000000003</v>
+      </c>
+      <c r="B49" s="2">
+        <v>-6.2704529999999998</v>
+      </c>
       <c r="C49">
         <v>27</v>
       </c>
@@ -1436,7 +1461,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="3:6">
+    <row r="50" spans="1:6" ht="15.75">
+      <c r="A50">
+        <v>53.338875000000002</v>
+      </c>
+      <c r="B50" s="2">
+        <v>-6.2754760000000003</v>
+      </c>
       <c r="C50">
         <v>27</v>
       </c>
@@ -1450,7 +1481,13 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="3:6">
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>53.338743999999998</v>
+      </c>
+      <c r="B51">
+        <v>-6.2784659999999999</v>
+      </c>
       <c r="C51">
         <v>27</v>
       </c>
@@ -1464,7 +1501,13 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="3:6">
+    <row r="52" spans="1:6">
+      <c r="A52">
+        <v>53.338354000000002</v>
+      </c>
+      <c r="B52">
+        <v>-6.2808159999999997</v>
+      </c>
       <c r="C52">
         <v>27</v>
       </c>
@@ -1478,7 +1521,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="3:6">
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>53.337532000000003</v>
+      </c>
+      <c r="B53">
+        <v>-6.2852290000000002</v>
+      </c>
       <c r="C53">
         <v>27</v>
       </c>
@@ -1492,7 +1541,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="3:6">
+    <row r="54" spans="1:6">
+      <c r="A54">
+        <v>53.334747999999998</v>
+      </c>
+      <c r="B54">
+        <v>-6.2897449999999999</v>
+      </c>
       <c r="C54">
         <v>27</v>
       </c>
@@ -1506,7 +1561,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="3:6">
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>53.333154999999998</v>
+      </c>
+      <c r="B55">
+        <v>-6.2916850000000002</v>
+      </c>
       <c r="C55">
         <v>27</v>
       </c>
@@ -1520,7 +1581,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="3:6">
+    <row r="56" spans="1:6" ht="15.75">
+      <c r="A56">
+        <v>53.331502999999998</v>
+      </c>
+      <c r="B56" s="2">
+        <v>-6.294556</v>
+      </c>
       <c r="C56">
         <v>27</v>
       </c>
@@ -1534,7 +1601,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="3:6">
+    <row r="57" spans="1:6" ht="15.75">
+      <c r="A57">
+        <v>53.330376000000001</v>
+      </c>
+      <c r="B57" s="2">
+        <v>-6.2974459999999999</v>
+      </c>
       <c r="C57">
         <v>27</v>
       </c>
@@ -1548,7 +1621,13 @@
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="3:6">
+    <row r="58" spans="1:6" ht="15.75">
+      <c r="A58">
+        <v>53.329031999999998</v>
+      </c>
+      <c r="B58" s="2">
+        <v>-6.3024519999999997</v>
+      </c>
       <c r="C58">
         <v>27</v>
       </c>
@@ -1562,7 +1641,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="3:6">
+    <row r="59" spans="1:6" ht="15.75">
+      <c r="A59">
+        <v>53.328077999999998</v>
+      </c>
+      <c r="B59" s="2">
+        <v>-6.306794</v>
+      </c>
       <c r="C59">
         <v>27</v>
       </c>
@@ -1576,7 +1661,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="3:6">
+    <row r="60" spans="1:6" ht="15.75">
+      <c r="A60">
+        <v>53.327423000000003</v>
+      </c>
+      <c r="B60" s="2">
+        <v>-6.3097159999999999</v>
+      </c>
       <c r="C60">
         <v>27</v>
       </c>
@@ -1590,7 +1681,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="3:6">
+    <row r="61" spans="1:6" ht="15.75">
+      <c r="A61" s="2">
+        <v>53.325555000000001</v>
+      </c>
+      <c r="B61" s="2">
+        <v>-6.3165829999999996</v>
+      </c>
       <c r="C61">
         <v>27</v>
       </c>
@@ -1604,7 +1701,13 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="3:6">
+    <row r="62" spans="1:6" ht="15.75">
+      <c r="A62" s="2">
+        <v>53.324928</v>
+      </c>
+      <c r="B62" s="2">
+        <v>-6.3182119999999999</v>
+      </c>
       <c r="C62">
         <v>27</v>
       </c>
@@ -1618,7 +1721,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="3:6">
+    <row r="63" spans="1:6" ht="15.75">
+      <c r="A63" s="2">
+        <v>53.324235000000002</v>
+      </c>
+      <c r="B63" s="2">
+        <v>-6.3262140000000002</v>
+      </c>
       <c r="C63">
         <v>27</v>
       </c>
@@ -1632,7 +1741,13 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="3:6">
+    <row r="64" spans="1:6" ht="15.75">
+      <c r="A64" s="2">
+        <v>53.32208</v>
+      </c>
+      <c r="B64" s="2">
+        <v>-6.3299750000000001</v>
+      </c>
       <c r="C64">
         <v>27</v>
       </c>
@@ -1646,7 +1761,13 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="3:6">
+    <row r="65" spans="1:6" ht="15.75">
+      <c r="A65" s="2">
+        <v>53.321055999999999</v>
+      </c>
+      <c r="B65" s="2">
+        <v>-6.3309420000000003</v>
+      </c>
       <c r="C65">
         <v>27</v>
       </c>
@@ -1660,7 +1781,13 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" spans="3:6">
+    <row r="66" spans="1:6" ht="15.75">
+      <c r="A66" s="2">
+        <v>53.317833999999998</v>
+      </c>
+      <c r="B66" s="2">
+        <v>-6.3326469999999997</v>
+      </c>
       <c r="C66">
         <v>27</v>
       </c>
@@ -1674,7 +1801,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="3:6">
+    <row r="67" spans="1:6" ht="15.75">
+      <c r="A67" s="2">
+        <v>53.315530000000003</v>
+      </c>
+      <c r="B67" s="2">
+        <v>-6.3347319999999998</v>
+      </c>
       <c r="C67">
         <v>27</v>
       </c>
@@ -1688,7 +1821,13 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="3:6">
+    <row r="68" spans="1:6" ht="15.75">
+      <c r="A68" s="2">
+        <v>53.313304000000002</v>
+      </c>
+      <c r="B68" s="2">
+        <v>-6.3412110000000004</v>
+      </c>
       <c r="C68">
         <v>27</v>
       </c>
@@ -1702,7 +1841,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="3:6">
+    <row r="69" spans="1:6" ht="15.75">
+      <c r="A69" s="2">
+        <v>53.311644999999999</v>
+      </c>
+      <c r="B69" s="2">
+        <v>-6.3431090000000001</v>
+      </c>
       <c r="C69">
         <v>27</v>
       </c>
@@ -1716,7 +1861,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="3:6">
+    <row r="70" spans="1:6" ht="15.75">
+      <c r="A70" s="2">
+        <v>53.308857000000003</v>
+      </c>
+      <c r="B70" s="2">
+        <v>-6.3457369999999997</v>
+      </c>
       <c r="C70">
         <v>27</v>
       </c>
@@ -1730,7 +1881,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="71" spans="3:6">
+    <row r="71" spans="1:6" ht="15.75">
+      <c r="A71" s="2">
+        <v>53.305979999999998</v>
+      </c>
+      <c r="B71" s="2">
+        <v>-6.3485060000000004</v>
+      </c>
       <c r="C71">
         <v>27</v>
       </c>
@@ -1744,7 +1901,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="3:6">
+    <row r="72" spans="1:6" ht="15.75">
+      <c r="A72" s="2">
+        <v>53.302568999999998</v>
+      </c>
+      <c r="B72" s="2">
+        <v>-6.3514939999999998</v>
+      </c>
       <c r="C72">
         <v>27</v>
       </c>
@@ -1758,7 +1921,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="3:6">
+    <row r="73" spans="1:6" ht="15.75">
+      <c r="A73" s="2">
+        <v>53.300631000000003</v>
+      </c>
+      <c r="B73" s="2">
+        <v>-6.353091</v>
+      </c>
       <c r="C73">
         <v>27</v>
       </c>
@@ -1772,7 +1941,13 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="3:6">
+    <row r="74" spans="1:6" ht="15.75">
+      <c r="A74" s="2">
+        <v>53.297431000000003</v>
+      </c>
+      <c r="B74" s="2">
+        <v>-6.3542249999999996</v>
+      </c>
       <c r="C74">
         <v>27</v>
       </c>
@@ -1786,7 +1961,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="3:6">
+    <row r="75" spans="1:6" ht="15.75">
+      <c r="A75" s="2">
+        <v>53.294001999999999</v>
+      </c>
+      <c r="B75" s="2">
+        <v>-6.3555029999999997</v>
+      </c>
       <c r="C75">
         <v>27</v>
       </c>
@@ -1800,7 +1981,13 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="3:6">
+    <row r="76" spans="1:6" ht="15.75">
+      <c r="A76" s="2">
+        <v>53.289245999999999</v>
+      </c>
+      <c r="B76" s="2">
+        <v>-6.3576040000000003</v>
+      </c>
       <c r="C76">
         <v>27</v>
       </c>
@@ -1814,7 +2001,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="3:6">
+    <row r="77" spans="1:6">
+      <c r="A77">
+        <v>53.288500999999997</v>
+      </c>
+      <c r="B77">
+        <v>-6.3632749999999998</v>
+      </c>
       <c r="C77">
         <v>27</v>
       </c>
@@ -1828,7 +2021,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="3:6">
+    <row r="78" spans="1:6" ht="15.75">
+      <c r="A78" s="2">
+        <v>53.289222000000002</v>
+      </c>
+      <c r="B78" s="2">
+        <v>6.3670280000000004</v>
+      </c>
       <c r="C78">
         <v>27</v>
       </c>
@@ -1842,7 +2041,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="3:6">
+    <row r="79" spans="1:6" ht="15.75">
+      <c r="A79" s="2">
+        <v>53.290438999999999</v>
+      </c>
+      <c r="B79" s="2">
+        <v>-6.3693400000000002</v>
+      </c>
       <c r="C79">
         <v>27</v>
       </c>
@@ -1856,7 +2061,13 @@
         <v>95</v>
       </c>
     </row>
-    <row r="80" spans="3:6">
+    <row r="80" spans="1:6" ht="15.75">
+      <c r="A80" s="2">
+        <v>53.289386</v>
+      </c>
+      <c r="B80" s="2">
+        <v>-6.373729</v>
+      </c>
       <c r="C80">
         <v>27</v>
       </c>
@@ -1870,7 +2081,13 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="3:6">
+    <row r="81" spans="1:6" ht="15.75">
+      <c r="A81" s="2">
+        <v>53.286414999999998</v>
+      </c>
+      <c r="B81" s="2">
+        <v>-6.3749229999999999</v>
+      </c>
       <c r="C81">
         <v>27</v>
       </c>
@@ -1884,7 +2101,13 @@
         <v>98</v>
       </c>
     </row>
-    <row r="82" spans="3:6">
+    <row r="82" spans="1:6" ht="15.75">
+      <c r="A82" s="2">
+        <v>53.285026999999999</v>
+      </c>
+      <c r="B82" s="2">
+        <v>-6.37852</v>
+      </c>
       <c r="C82">
         <v>27</v>
       </c>
@@ -1898,7 +2121,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="83" spans="3:6">
+    <row r="83" spans="1:6" ht="15.75">
+      <c r="A83" s="2">
+        <v>53.283195999999997</v>
+      </c>
+      <c r="B83" s="2">
+        <v>-6.384512</v>
+      </c>
       <c r="C83">
         <v>27</v>
       </c>
@@ -1912,7 +2141,13 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="3:6">
+    <row r="84" spans="1:6" ht="15.75">
+      <c r="A84" s="2">
+        <v>53.282167000000001</v>
+      </c>
+      <c r="B84" s="2">
+        <v>-6.3895479999999996</v>
+      </c>
       <c r="C84">
         <v>27</v>
       </c>
@@ -1926,7 +2161,13 @@
         <v>103</v>
       </c>
     </row>
-    <row r="85" spans="3:6">
+    <row r="85" spans="1:6" ht="15.75">
+      <c r="A85" s="2">
+        <v>53.283799999999999</v>
+      </c>
+      <c r="B85" s="2">
+        <v>-6.3925850000000004</v>
+      </c>
       <c r="C85">
         <v>27</v>
       </c>
@@ -1940,7 +2181,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="3:6">
+    <row r="86" spans="1:6" ht="15.75">
+      <c r="A86" s="2">
+        <v>53.285522999999998</v>
+      </c>
+      <c r="B86" s="2">
+        <v>-6.3949020000000001</v>
+      </c>
       <c r="C86">
         <v>27</v>
       </c>
@@ -1954,7 +2201,13 @@
         <v>107</v>
       </c>
     </row>
-    <row r="87" spans="3:6">
+    <row r="87" spans="1:6" ht="15.75">
+      <c r="A87" s="2">
+        <v>53.288755999999999</v>
+      </c>
+      <c r="B87" s="2">
+        <v>-6.400163</v>
+      </c>
       <c r="C87">
         <v>27</v>
       </c>
@@ -1968,7 +2221,13 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="3:6">
+    <row r="88" spans="1:6" ht="15.75">
+      <c r="A88" s="2">
+        <v>53.288522999999998</v>
+      </c>
+      <c r="B88" s="2">
+        <v>-6.4045829999999997</v>
+      </c>
       <c r="C88">
         <v>27</v>
       </c>
@@ -1982,7 +2241,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="89" spans="3:6">
+    <row r="89" spans="1:6" ht="15.75">
+      <c r="A89" s="2">
+        <v>53.285913000000001</v>
+      </c>
+      <c r="B89" s="2">
+        <v>-6.4073149999999996</v>
+      </c>
       <c r="C89">
         <v>27</v>
       </c>
@@ -1996,7 +2261,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="90" spans="3:6">
+    <row r="90" spans="1:6" ht="15.75">
+      <c r="A90" s="2">
+        <v>53.285024999999997</v>
+      </c>
+      <c r="B90" s="2">
+        <v>-6.4062330000000003</v>
+      </c>
       <c r="C90">
         <v>27</v>
       </c>
@@ -2010,7 +2281,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="91" spans="3:6">
+    <row r="91" spans="1:6" ht="15.75">
+      <c r="A91" s="2">
+        <v>53.282865999999999</v>
+      </c>
+      <c r="B91" s="2">
+        <v>-6.4017980000000003</v>
+      </c>
       <c r="C91">
         <v>27</v>
       </c>
@@ -2024,7 +2301,13 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="3:6">
+    <row r="92" spans="1:6" ht="15.75">
+      <c r="A92" s="2">
+        <v>53.280836999999998</v>
+      </c>
+      <c r="B92" s="2">
+        <v>-6.4034110000000002</v>
+      </c>
       <c r="C92">
         <v>27</v>
       </c>
@@ -2038,7 +2321,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="3:6">
+    <row r="93" spans="1:6">
       <c r="C93">
         <v>27</v>
       </c>

</xml_diff>